<commit_message>
refactor: esquema de vacunación en country_data.General de select a free text.
</commit_message>
<xml_diff>
--- a/template/ENG/country_data.xlsx
+++ b/template/ENG/country_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk-assessment/template/ENG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CF99AF-369C-7342-94AC-1C20F85EB6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A1CDAA-07EA-024C-8F68-B9511E36EF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28620" windowHeight="15980" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
   </bookViews>
@@ -1094,9 +1094,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1134,7 +1134,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1240,7 +1240,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1382,7 +1382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1448,18 +1448,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BC92D02-843F-244F-9460-E090EF2C7C0A}">
-          <x14:formula1>
-            <xm:f>_ListValues!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>